<commit_message>
Minor tweaks to simplify age bias correction
</commit_message>
<xml_diff>
--- a/data/SAD0_36.xlsx
+++ b/data/SAD0_36.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Harpseals/HSmodel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EEBDEA1-E288-47DF-A85C-84AD1BC01C5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{0EEBDEA1-E288-47DF-A85C-84AD1BC01C5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8B8BB788-ADC9-48D9-A045-5B272BF4DD77}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="1650" windowWidth="19995" windowHeight="12480"/>
+    <workbookView xWindow="29610" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAD0_36" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -865,14 +865,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -880,292 +882,292 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9.32012510602441E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+        <v>9.6476606000000006E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>8.0640892108540002E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+        <v>8.2428554000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7.0962574864674596E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+        <v>7.1943749000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>6.3181235370138006E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+        <v>6.3603134000000006E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5.6640838654682002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+        <v>5.6778598E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>5.1216129072201202E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+        <v>5.1076533E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.6561194927936499E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+        <v>4.6236073000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.2547149655753097E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+        <v>4.2074571999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3.9016135591067598E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+        <v>3.8452368000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3.5884014297301203E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
+        <v>3.5252987E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>3.3057748157674302E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
+        <v>3.2379460999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3.0456113087830399E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
+        <v>2.9757838000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2.8065988730936402E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
+        <v>2.7346947E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2.5889215647073398E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
+        <v>2.5158990999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2.4028865712441099E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+        <v>2.3276809999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>2.2410855089447901E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
+        <v>2.169455E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2.0961329795277799E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+        <v>2.0293176E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1.9605839993825199E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.9023919E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1.8361954810760198E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.7946446000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>2.3416700781752099E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
+        <v>2.3286067000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>2.1403039996155102E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
+        <v>2.1274210000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>1.9546542178963101E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.9445661E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1.78568553697174E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.7761559E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1.6264135265360101E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.6203492999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1.47930883220812E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.4755971E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>1.34335844155199E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.3405158E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1.21821365740467E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.2137317E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>1.0953313904719699E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.5">
+        <v>1.0936708E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>9.7903647653384204E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
+        <v>9.7851799999999992E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>8.6461391880656296E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
+        <v>8.6647670000000003E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>7.5159810646262303E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
+        <v>7.5615320000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>6.3842738506162001E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.5">
+        <v>6.4687579999999998E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>5.26174864987085E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.5">
+        <v>5.392099E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>4.1738102284066703E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.5">
+        <v>4.3530590000000003E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <v>3.1382138432966898E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.5">
+        <v>3.3637049999999998E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <v>2.5507449736590598E-3</v>
+        <v>4.0034440000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>